<commit_message>
Copes when named references contain table references
</commit_message>
<xml_diff>
--- a/examples/keepingtables.xlsx
+++ b/examples/keepingtables.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="620" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="named_reference_to_table">Table1[#All]</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>name</t>
   </si>
@@ -46,6 +49,12 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>named_reference_to_table</t>
+  </si>
+  <si>
+    <t>=Table1[#All]</t>
   </si>
 </sst>
 </file>
@@ -58,6 +67,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -436,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:D13"/>
+  <dimension ref="C4:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="4" spans="3:4">
+    <row r="4" spans="3:7">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -452,7 +462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:4">
+    <row r="5" spans="3:7">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -460,7 +470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:4">
+    <row r="6" spans="3:7">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -468,15 +478,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:4">
+    <row r="7" spans="3:7">
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="3:4">
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7">
       <c r="C10" t="s">
         <v>0</v>
       </c>
@@ -484,7 +500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="3:4">
+    <row r="11" spans="3:7">
       <c r="C11" t="s">
         <v>6</v>
       </c>
@@ -493,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="3:4">
+    <row r="12" spans="3:7">
       <c r="C12" t="s">
         <v>7</v>
       </c>
@@ -502,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:4">
+    <row r="13" spans="3:7">
       <c r="C13" t="s">
         <v>8</v>
       </c>

</xml_diff>